<commit_message>
final changes done ready to be published
</commit_message>
<xml_diff>
--- a/FoodTracker.xlsx
+++ b/FoodTracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhautik/Desktop/Winter Arc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26214E76-F2E3-3A42-9366-2D8C8F792B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79485B1-C83F-D041-9192-F7B5960985BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="213">
   <si>
     <t>Date</t>
   </si>
@@ -644,9 +644,6 @@
     <t>318.3,153.6,83.7</t>
   </si>
   <si>
-    <t>88.3,52.2,25.6</t>
-  </si>
-  <si>
     <t>Haldiram Mung Daal + Aloo Bhujiya</t>
   </si>
   <si>
@@ -663,6 +660,18 @@
   </si>
   <si>
     <t>84.4,19.2,29.5</t>
+  </si>
+  <si>
+    <t>(H)Pigeon peas Dal with Protien tortillas, peanuts</t>
+  </si>
+  <si>
+    <t>90.0,54,35.8</t>
+  </si>
+  <si>
+    <t>236.6,153.4,82.4</t>
+  </si>
+  <si>
+    <t>264.7,150.4,91.9</t>
   </si>
 </sst>
 </file>
@@ -1035,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L2" zoomScale="131" workbookViewId="0">
-      <selection activeCell="AD29" sqref="AD29"/>
+    <sheetView tabSelected="1" topLeftCell="X4" zoomScale="131" workbookViewId="0">
+      <selection activeCell="AG29" sqref="AG29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1211,7 +1220,7 @@
         <v>494</v>
       </c>
       <c r="L2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M2" t="s">
         <v>42</v>
@@ -1316,7 +1325,7 @@
         <v>840</v>
       </c>
       <c r="AF3">
-        <f t="shared" ref="AF3:AF28" si="0">AD3-AE3</f>
+        <f t="shared" ref="AF3:AF29" si="0">AD3-AE3</f>
         <v>1459</v>
       </c>
       <c r="AG3">
@@ -3643,10 +3652,10 @@
         <v>557</v>
       </c>
       <c r="F28" t="s">
+        <v>204</v>
+      </c>
+      <c r="G28" t="s">
         <v>205</v>
-      </c>
-      <c r="G28" t="s">
-        <v>206</v>
       </c>
       <c r="H28">
         <v>563</v>
@@ -3655,7 +3664,7 @@
         <v>141</v>
       </c>
       <c r="J28" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K28">
         <v>714</v>
@@ -3722,7 +3731,7 @@
         <v>13518</v>
       </c>
       <c r="AI28" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.2">
@@ -3744,19 +3753,19 @@
         <v>557</v>
       </c>
       <c r="F29" t="s">
+        <v>207</v>
+      </c>
+      <c r="G29" t="s">
         <v>208</v>
-      </c>
-      <c r="G29" t="s">
-        <v>209</v>
       </c>
       <c r="H29">
         <v>686</v>
       </c>
       <c r="I29" t="s">
-        <v>129</v>
+        <v>209</v>
       </c>
       <c r="J29" t="s">
-        <v>130</v>
+        <v>210</v>
       </c>
       <c r="K29">
         <v>786</v>
@@ -3789,19 +3798,32 @@
         <v>120</v>
       </c>
       <c r="AA29">
-        <v>263.89999999999998</v>
+        <v>264.7</v>
       </c>
       <c r="AB29">
-        <v>141.9</v>
+        <v>150.4</v>
       </c>
       <c r="AC29">
-        <v>88.3</v>
+        <v>91.9</v>
       </c>
       <c r="AD29">
-        <v>557</v>
+        <v>2059</v>
+      </c>
+      <c r="AE29">
+        <v>1089</v>
+      </c>
+      <c r="AF29">
+        <f t="shared" si="0"/>
+        <v>970</v>
+      </c>
+      <c r="AG29">
+        <v>3</v>
+      </c>
+      <c r="AH29">
+        <v>16719</v>
       </c>
       <c r="AI29" t="s">
-        <v>48</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>